<commit_message>
Added half of the 24hr results, still feature selection left
</commit_message>
<xml_diff>
--- a/results/24hr_KNN.xlsx
+++ b/results/24hr_KNN.xlsx
@@ -409,7 +409,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C6" activeCellId="0" pane="topLeft" sqref="A2:C6"/>
@@ -446,6 +446,17 @@
         <v>0.717</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.717</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>

</xml_diff>